<commit_message>
adding fix to data dictionary and preprocessing
</commit_message>
<xml_diff>
--- a/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
+++ b/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/Data/Preprocessed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A02B18-FD1E-5C42-8BED-7C47326BD387}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E468B-D70F-E44C-9D8A-BA7BA1DD0E1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
   </bookViews>
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updating escape data preprocessing to fix lab units
</commit_message>
<xml_diff>
--- a/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
+++ b/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/Data/Preprocessed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E468B-D70F-E44C-9D8A-BA7BA1DD0E1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B29B57F-B678-8D41-8F7B-CC302CEC9E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="245">
   <si>
     <t>*Bold is the category name, underneath is the parameters in that section</t>
   </si>
@@ -760,9 +760,6 @@
     <t>Distance in Feet</t>
   </si>
   <si>
-    <t>g/L</t>
-  </si>
-  <si>
     <t>U/L</t>
   </si>
   <si>
@@ -850,6 +847,12 @@
   </si>
   <si>
     <t>mL/kg/min</t>
+  </si>
+  <si>
+    <t>10^9/L</t>
+  </si>
+  <si>
+    <t>&lt;- note these same</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,10 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,22 +1272,22 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1294,7 +1300,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1327,7 +1333,7 @@
         <v>211</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -1703,13 +1709,13 @@
         <v>218</v>
       </c>
       <c r="C46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="19" x14ac:dyDescent="0.2">
@@ -2166,7 +2172,7 @@
         <v>220</v>
       </c>
       <c r="E91" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H91" t="s">
         <v>100</v>
@@ -2180,7 +2186,7 @@
         <v>213</v>
       </c>
       <c r="E92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -2199,10 +2205,10 @@
         <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="D95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H95" t="s">
         <v>104</v>
@@ -2213,10 +2219,10 @@
         <v>105</v>
       </c>
       <c r="B96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H96" t="s">
         <v>106</v>
@@ -2227,10 +2233,10 @@
         <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D97" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H97" t="s">
         <v>108</v>
@@ -2241,16 +2247,22 @@
         <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E98" t="s">
-        <v>223</v>
+        <v>222</v>
+      </c>
+      <c r="F98" t="s">
+        <v>222</v>
+      </c>
+      <c r="G98" t="s">
+        <v>222</v>
       </c>
       <c r="H98" t="s">
         <v>110</v>
@@ -2261,16 +2273,22 @@
         <v>111</v>
       </c>
       <c r="B99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E99" t="s">
-        <v>223</v>
+        <v>222</v>
+      </c>
+      <c r="F99" t="s">
+        <v>222</v>
+      </c>
+      <c r="G99" t="s">
+        <v>222</v>
       </c>
       <c r="H99" t="s">
         <v>112</v>
@@ -2281,7 +2299,7 @@
         <v>113</v>
       </c>
       <c r="B100" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H100" t="s">
         <v>114</v>
@@ -2295,7 +2313,7 @@
         <v>215</v>
       </c>
       <c r="C101" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H101" t="s">
         <v>116</v>
@@ -2306,10 +2324,10 @@
         <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C102" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H102" t="s">
         <v>118</v>
@@ -2320,13 +2338,16 @@
         <v>119</v>
       </c>
       <c r="B103" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C103" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D103" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="E103" t="s">
+        <v>244</v>
       </c>
       <c r="H103" t="s">
         <v>120</v>
@@ -2337,13 +2358,16 @@
         <v>121</v>
       </c>
       <c r="B104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D104" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="E104" t="s">
+        <v>244</v>
       </c>
       <c r="H104" t="s">
         <v>122</v>
@@ -2354,13 +2378,19 @@
         <v>123</v>
       </c>
       <c r="B105" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C105" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D105" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="F105" t="s">
+        <v>224</v>
+      </c>
+      <c r="G105" t="s">
+        <v>224</v>
       </c>
       <c r="H105" t="s">
         <v>124</v>
@@ -2371,10 +2401,10 @@
         <v>125</v>
       </c>
       <c r="B106" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D106" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H106" t="s">
         <v>126</v>
@@ -2385,10 +2415,10 @@
         <v>127</v>
       </c>
       <c r="B107" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="D107" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H107" t="s">
         <v>128</v>
@@ -2399,13 +2429,19 @@
         <v>129</v>
       </c>
       <c r="B108" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C108" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D108" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="F108" t="s">
+        <v>243</v>
+      </c>
+      <c r="G108" t="s">
+        <v>243</v>
       </c>
       <c r="H108" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Updating all data preprocessing to fix lab units
</commit_message>
<xml_diff>
--- a/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
+++ b/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/Data/Preprocessed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B29B57F-B678-8D41-8F7B-CC302CEC9E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42924322-BD7F-5A44-AE8E-13D5801F1B3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="246">
   <si>
     <t>*Bold is the category name, underneath is the parameters in that section</t>
   </si>
@@ -853,6 +853,9 @@
   </si>
   <si>
     <t>&lt;- note these same</t>
+  </si>
+  <si>
+    <t>1 male, 2 female</t>
   </si>
 </sst>
 </file>
@@ -1230,13 +1233,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32E90D8-0482-BA4B-B75F-C9DD8C8422E0}">
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,62 +1303,56 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>210</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" t="s">
-        <v>228</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>212</v>
@@ -1364,873 +1361,873 @@
         <v>212</v>
       </c>
       <c r="H12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>212</v>
-      </c>
-      <c r="H15" t="s">
-        <v>3</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>212</v>
       </c>
       <c r="H16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>212</v>
       </c>
       <c r="H17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>212</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>212</v>
       </c>
       <c r="H19" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>213</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>214</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>215</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>212</v>
-      </c>
-      <c r="H25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>212</v>
       </c>
       <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>212</v>
+      </c>
+      <c r="H27" t="s">
         <v>28</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>216</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>31</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I28" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>212</v>
-      </c>
-      <c r="H28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
         <v>212</v>
       </c>
       <c r="H29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>212</v>
       </c>
       <c r="H30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>212</v>
+      </c>
+      <c r="H31" t="s">
         <v>40</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
       <c r="H33" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>44</v>
       </c>
       <c r="H34" t="s">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s">
-        <v>185</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="I35" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>176</v>
-      </c>
-      <c r="B36" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="H36" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="H37" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>207</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>182</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I38" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>218</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>229</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>236</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" t="s">
-        <v>215</v>
-      </c>
-      <c r="H48" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>215</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>71</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" t="s">
-        <v>208</v>
-      </c>
-      <c r="H53" t="s">
-        <v>67</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
         <v>208</v>
       </c>
       <c r="H54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>208</v>
+      </c>
+      <c r="H55" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>205</v>
-      </c>
-      <c r="B57" t="s">
-        <v>209</v>
-      </c>
-      <c r="H57" t="s">
-        <v>188</v>
-      </c>
-      <c r="I57" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>205</v>
+      </c>
+      <c r="B58" t="s">
+        <v>209</v>
+      </c>
+      <c r="H58" t="s">
+        <v>188</v>
+      </c>
+      <c r="I58" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>206</v>
       </c>
-      <c r="B58" t="s">
-        <v>209</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="B59" t="s">
+        <v>209</v>
+      </c>
+      <c r="H59" t="s">
         <v>190</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I59" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" t="s">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" t="s">
-        <v>209</v>
-      </c>
-      <c r="H61" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
         <v>209</v>
       </c>
       <c r="H62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
         <v>209</v>
       </c>
       <c r="H63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
         <v>209</v>
       </c>
       <c r="H64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
         <v>209</v>
       </c>
       <c r="H65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
         <v>209</v>
       </c>
       <c r="H66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
         <v>209</v>
       </c>
       <c r="H67" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
         <v>209</v>
       </c>
       <c r="H68" t="s">
-        <v>162</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
         <v>209</v>
       </c>
       <c r="H69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
         <v>209</v>
       </c>
       <c r="H70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
         <v>209</v>
       </c>
       <c r="H71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
         <v>209</v>
       </c>
       <c r="H72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
         <v>209</v>
       </c>
       <c r="H73" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
         <v>209</v>
       </c>
       <c r="H74" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>204</v>
       </c>
       <c r="B75" t="s">
         <v>209</v>
       </c>
       <c r="H75" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
         <v>209</v>
       </c>
       <c r="H76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
         <v>209</v>
       </c>
       <c r="H77" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s">
         <v>209</v>
       </c>
       <c r="H78" t="s">
-        <v>200</v>
-      </c>
-      <c r="I78" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
         <v>209</v>
       </c>
       <c r="H79" t="s">
-        <v>173</v>
+        <v>200</v>
+      </c>
+      <c r="I79" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
         <v>209</v>
       </c>
       <c r="H80" t="s">
-        <v>197</v>
-      </c>
-      <c r="I80" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>198</v>
+      </c>
+      <c r="B81" t="s">
+        <v>209</v>
+      </c>
+      <c r="H81" t="s">
+        <v>197</v>
+      </c>
+      <c r="I81" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>194</v>
       </c>
-      <c r="B81" t="s">
-        <v>209</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="B82" t="s">
+        <v>209</v>
+      </c>
+      <c r="H82" t="s">
         <v>195</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I82" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>78</v>
-      </c>
-      <c r="B84" t="s">
-        <v>209</v>
-      </c>
-      <c r="H84" t="s">
-        <v>175</v>
-      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
         <v>209</v>
       </c>
       <c r="H85" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
         <v>209</v>
       </c>
       <c r="H86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
         <v>209</v>
       </c>
       <c r="H87" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>209</v>
+      </c>
+      <c r="H88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>91</v>
       </c>
-      <c r="B88" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+      <c r="B89" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>99</v>
-      </c>
-      <c r="B91" t="s">
-        <v>220</v>
-      </c>
-      <c r="E91" t="s">
-        <v>241</v>
-      </c>
-      <c r="H91" t="s">
-        <v>100</v>
-      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" t="s">
+        <v>241</v>
+      </c>
+      <c r="H92" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>101</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>213</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>103</v>
-      </c>
-      <c r="B95" t="s">
-        <v>231</v>
-      </c>
-      <c r="D95" t="s">
-        <v>231</v>
-      </c>
-      <c r="H95" t="s">
-        <v>104</v>
-      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="D96" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="H96" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
         <v>221</v>
@@ -2239,38 +2236,26 @@
         <v>221</v>
       </c>
       <c r="H97" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
-      </c>
-      <c r="C98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D98" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" t="s">
-        <v>222</v>
-      </c>
-      <c r="F98" t="s">
-        <v>222</v>
-      </c>
-      <c r="G98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H98" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B99" t="s">
         <v>222</v>
@@ -2291,91 +2276,97 @@
         <v>222</v>
       </c>
       <c r="H99" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
         <v>222</v>
       </c>
+      <c r="C100" t="s">
+        <v>222</v>
+      </c>
+      <c r="D100" t="s">
+        <v>222</v>
+      </c>
+      <c r="E100" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" t="s">
+        <v>222</v>
+      </c>
+      <c r="G100" t="s">
+        <v>222</v>
+      </c>
       <c r="H100" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B101" t="s">
-        <v>215</v>
-      </c>
-      <c r="C101" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H101" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>115</v>
+      </c>
+      <c r="B102" t="s">
+        <v>215</v>
+      </c>
+      <c r="C102" t="s">
+        <v>230</v>
+      </c>
+      <c r="H102" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>117</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>231</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>231</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H103" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="19" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+    <row r="104" spans="1:10" ht="19" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>119</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>223</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>232</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>237</v>
-      </c>
-      <c r="E103" t="s">
-        <v>244</v>
-      </c>
-      <c r="H103" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>121</v>
-      </c>
-      <c r="B104" t="s">
-        <v>224</v>
-      </c>
-      <c r="C104" t="s">
-        <v>224</v>
-      </c>
-      <c r="D104" t="s">
-        <v>238</v>
       </c>
       <c r="E104" t="s">
         <v>244</v>
       </c>
       <c r="H104" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B105" t="s">
         <v>224</v>
@@ -2386,119 +2377,122 @@
       <c r="D105" t="s">
         <v>238</v>
       </c>
-      <c r="F105" t="s">
-        <v>224</v>
-      </c>
-      <c r="G105" t="s">
-        <v>224</v>
+      <c r="E105" t="s">
+        <v>244</v>
       </c>
       <c r="H105" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B106" t="s">
-        <v>222</v>
+        <v>224</v>
+      </c>
+      <c r="C106" t="s">
+        <v>224</v>
       </c>
       <c r="D106" t="s">
-        <v>222</v>
+        <v>238</v>
+      </c>
+      <c r="F106" t="s">
+        <v>224</v>
+      </c>
+      <c r="G106" t="s">
+        <v>224</v>
       </c>
       <c r="H106" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" t="s">
+        <v>222</v>
+      </c>
+      <c r="D107" t="s">
+        <v>222</v>
+      </c>
+      <c r="H107" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>127</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>231</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>231</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H108" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="19" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="109" spans="1:10" ht="19" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>129</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>223</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>233</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" t="s">
         <v>237</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F109" t="s">
         <v>243</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G109" t="s">
         <v>243</v>
       </c>
-      <c r="H108" t="s">
+      <c r="H109" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-    </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-      <c r="I110" t="s">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="I111" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B111" t="s">
-        <v>209</v>
-      </c>
-      <c r="H111" t="s">
-        <v>143</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J111" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B112" t="s">
         <v>209</v>
       </c>
       <c r="H112" t="s">
-        <v>135</v>
-      </c>
-      <c r="I112" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="J112" t="s">
         <v>140</v>
@@ -2506,16 +2500,16 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B113" t="s">
         <v>209</v>
       </c>
       <c r="H113" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I113" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J113" t="s">
         <v>140</v>
@@ -2523,147 +2517,164 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B114" t="s">
         <v>209</v>
       </c>
       <c r="H114" t="s">
-        <v>138</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="I114" t="s">
+        <v>145</v>
       </c>
       <c r="J114" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B115" t="s">
+        <v>209</v>
+      </c>
+      <c r="H115" t="s">
+        <v>138</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J115" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>147</v>
-      </c>
-      <c r="B117" t="s">
-        <v>211</v>
-      </c>
-      <c r="H117" t="s">
-        <v>21</v>
-      </c>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H118" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B119" t="s">
         <v>212</v>
       </c>
       <c r="H119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>149</v>
+      </c>
+      <c r="B120" t="s">
+        <v>212</v>
+      </c>
+      <c r="H120" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" t="s">
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4" t="s">
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="I122" s="4" t="s">
+      <c r="I123" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="J122" s="4"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>24</v>
-      </c>
-      <c r="H123" t="s">
-        <v>25</v>
-      </c>
-      <c r="I123" t="s">
-        <v>26</v>
-      </c>
+      <c r="J123" s="4"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H124" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I124" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>33</v>
+      </c>
+      <c r="H125" t="s">
+        <v>34</v>
+      </c>
+      <c r="I125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>36</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H126" t="s">
         <v>37</v>
       </c>
-      <c r="I125" t="s">
+      <c r="I126" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+    <row r="127" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>44</v>
       </c>
-      <c r="B126"/>
-      <c r="C126"/>
-      <c r="D126"/>
-      <c r="E126"/>
-      <c r="F126"/>
-      <c r="G126"/>
-      <c r="H126" t="s">
+      <c r="B127"/>
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="G127"/>
+      <c r="H127" t="s">
         <v>45</v>
       </c>
-      <c r="I126" t="s">
+      <c r="I127" t="s">
         <v>46</v>
       </c>
-      <c r="J126"/>
+      <c r="J127"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed updated All Feature training results
</commit_message>
<xml_diff>
--- a/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
+++ b/Data/Preprocessed Data/Data_Dictionary_UNITS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/Data/Preprocessed Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/CARNA/Data/Preprocessed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42924322-BD7F-5A44-AE8E-13D5801F1B3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF71F6A-0AA3-1C47-94F2-059C48D44FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
+    <workbookView xWindow="53040" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -913,12 +913,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,10 +1234,10 @@
   <dimension ref="A1:J127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E116" sqref="E116"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,14 +1577,9 @@
       <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
       <c r="H32" t="s">
         <v>15</v>
       </c>
@@ -1598,12 +1591,6 @@
       <c r="A33" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
       <c r="H33" t="s">
         <v>23</v>
       </c>
@@ -1697,15 +1684,9 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1733,14 +1714,9 @@
       <c r="A48" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
       <c r="H48" t="s">
         <v>64</v>
       </c>
@@ -2482,7 +2458,7 @@
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
+      <c r="A112" t="s">
         <v>133</v>
       </c>
       <c r="B112" t="s">
@@ -2491,7 +2467,7 @@
       <c r="H112" t="s">
         <v>143</v>
       </c>
-      <c r="I112" s="3" t="s">
+      <c r="I112" s="2" t="s">
         <v>146</v>
       </c>
       <c r="J112" t="s">
@@ -2499,7 +2475,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+      <c r="A113" t="s">
         <v>134</v>
       </c>
       <c r="B113" t="s">
@@ -2516,7 +2492,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
+      <c r="A114" t="s">
         <v>136</v>
       </c>
       <c r="B114" t="s">
@@ -2533,7 +2509,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+      <c r="A115" t="s">
         <v>137</v>
       </c>
       <c r="B115" t="s">
@@ -2542,7 +2518,7 @@
       <c r="H115" t="s">
         <v>138</v>
       </c>
-      <c r="I115" s="3" t="s">
+      <c r="I115" s="2" t="s">
         <v>141</v>
       </c>
       <c r="J115" t="s">
@@ -2608,22 +2584,15 @@
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
+      <c r="A123" t="s">
         <v>96</v>
       </c>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4" t="s">
+      <c r="H123" t="s">
         <v>152</v>
       </c>
-      <c r="I123" s="4" t="s">
+      <c r="I123" t="s">
         <v>153</v>
       </c>
-      <c r="J123" s="4"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
@@ -2658,23 +2627,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>44</v>
       </c>
-      <c r="B127"/>
-      <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
-      <c r="F127"/>
-      <c r="G127"/>
       <c r="H127" t="s">
         <v>45</v>
       </c>
       <c r="I127" t="s">
         <v>46</v>
       </c>
-      <c r="J127"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>